<commit_message>
RKK_junfu - 3414843012 업데이트
</commit_message>
<xml_diff>
--- a/Data/RKK_junfu - 3414843012/RKK_junfu - 3414843012.xlsx
+++ b/Data/RKK_junfu - 3414843012/RKK_junfu - 3414843012.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\RKK_junfu - 3414843012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9E8498-2CD3-4F40-9478-14CCB9E88431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14726681-0FDB-402E-A862-6378F6148C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F100" authorId="0" shapeId="0" xr:uid="{F569BB7E-D7E3-4721-A1E3-0E383EC9023C}">
+    <comment ref="F100" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -77,12 +77,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="E115" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-11에 새로 추가된 노드들 (17개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F115" authorId="0" shapeId="0" xr:uid="{3CBDF2B7-1F4F-4567-B189-45B73AF47E4A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-11에 새로 추가된 노드들 (17개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="506">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1482,21 +1508,21 @@
     <t>纳米纤维激活凝血机制，自动封闭伤口，开启修复治疗模式。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>나노 섬유가 혈액 응고를 촉진하여 상처를 자동으로 봉합하고 치료합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+AutoBleeding.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>나노 섬유가 혈액 응고를 촉진하여 상처를 자동으로 봉합하고 치료합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>AutoBleeding.label</t>
   </si>
   <si>
@@ -1515,21 +1541,21 @@
     <t>应对重大受伤情况，全面开启治愈医疗。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>심각한 부상 시 전면적인 치유 프로토콜을 활성화해 생존 가능성을 높입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+Visual_enhancement.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>심각한 부상 시 전면적인 치유 프로토콜을 활성화해 생존 가능성을 높입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Visual_enhancement.label</t>
   </si>
   <si>
@@ -1548,21 +1574,21 @@
     <t>全景补充协议提供目标视距和焦点捕捉功能，让用户视觉精确，犀利</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>전방위 인식 보조 시스템이 목표 가시거리 확보 및 초점 조절 기능을 제공하여, 착용자의 시야를 정밀하고 날카롭게 만듭니다. 사격 정확도와 근접 명중률이 향상됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+Breath_system.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>전방위 인식 보조 시스템이 목표 가시거리 확보 및 초점 조절 기능을 제공하여, 착용자의 시야를 정밀하고 날카롭게 만듭니다. 사격 정확도와 근접 명중률이 향상됩니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Breath_system.label</t>
   </si>
   <si>
@@ -1605,21 +1631,21 @@
     <t>来自于无尽星芒头盔设计图的现实增强系统，全景实时计算与皮层脑波接入，不仅能够提供各种计算分析指导服务，还让人精神抖擞，意气风发</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>'무한 성광 헬멧' 설계 기반의 증강 현실 시스템입니다. 실시간 전방위 연산 및 피질 뇌파 접속으로 다양한 분석/지침을 제공하며, 착용자의 정신을 고양시켜 활력을 불어넣습니다. 의식과 조작 능력이 향상됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+Augmented_Reality.stages.0.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>'무한 성광 헬멧' 설계 기반의 증강 현실 시스템입니다. 실시간 전방위 연산 및 피질 뇌파 접속으로 다양한 분석/지침을 제공하며, 착용자의 정신을 고양시켜 활력을 불어넣습니다. 의식과 조작 능력이 향상됩니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Augmented_Reality.stages.0.label</t>
   </si>
   <si>
@@ -1650,21 +1676,21 @@
     <t>引用小功率电流通过芯片的辅助倒流调节，刺激脑皮层提振精神</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>저출력 전류를 칩을 통해 뇌 피질에 흘려보내 정신을 고양시킵니다. 일시적인 무드 보너스를 제공하며 중독 위험은 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+EX.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>저출력 전류를 칩을 통해 뇌 피질에 흘려보내 정신을 고양시킵니다. 일시적인 무드 보너스를 제공하며 중독 위험은 없습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>EX.label</t>
   </si>
   <si>
@@ -1683,21 +1709,21 @@
     <t>维多利亚的先锋作战方案，速度！速度！还是速度！你丫的脚底抹油都没你这么慢!菜鸟!</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 선봉대 작전 교리: 속도! 속도! 오직 속도! 이봐, 신참! 맨발에 기름칠을 하고 달려도 너보단 빠르겠다!\n\n이동 속도가 대폭 향상됩니다. 방어력은 일반적인 수준입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HediffDef+deep_AI.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 선봉대 작전 교리: 속도! 속도! 오직 속도! 이봐, 신참! 맨발에 기름칠을 하고 달려도 너보단 빠르겠다!\n\n이동 속도가 대폭 향상됩니다. 방어력은 일반적인 수준입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>deep_AI.label</t>
   </si>
   <si>
@@ -1731,42 +1757,42 @@
     <t>维多利亚研究部</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 전투복</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ResearchProjectDef+RK_Victoria.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 전투복</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>RK_Victoria.description</t>
   </si>
   <si>
     <t>学习维多利亚目前研究的新玩意.\n\n维多利亚研究部门目前最新研究的纳米战甲技术，其原理来自人类所发掘的无尽星芒科技</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아의 최신 연구 과제를 확인하세요.\n\n빅토리아 연구부가 인류의 '무한 성광' 기술을 기반으로 개발한 최신 나노 전투복 기술입니다. 연구 완료 시 최상위 성능의 랫킨 전투복을 제작할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ApparelLayerDef+kuabao.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아의 최신 연구 과제를 확인하세요.\n\n빅토리아 연구부가 인류의 '무한 성광' 기술을 기반으로 개발한 최신 나노 전투복 기술입니다. 연구 완료 시 최상위 성능의 랫킨 전투복을 제작할 수 있습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>ApparelLayerDef</t>
   </si>
   <si>
@@ -1800,168 +1826,168 @@
     <t>枫叶军服</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 단풍잎 군복</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+fengye.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 단풍잎 군복</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>fengye.description</t>
   </si>
   <si>
     <t>由鼠族大师长眠生所定制的枫叶元素的军服，镶有落花枫叶的纹案，精致典雅</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생이 제작한 단풍잎 문양 군복입니다. 보기에는 좋지만, 방어 능력은 평범한 옷 수준입니다. 약간의 보온 효과가 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+fengyewaitao.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생이 제작한 단풍잎 문양 군복입니다. 보기에는 좋지만, 방어 능력은 평범한 옷 수준입니다. 약간의 보온 효과가 있습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>fengyewaitao.label</t>
   </si>
   <si>
     <t>枫叶毛绒保暖小西服</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 단풍잎 솜털 방한 미니 슈트</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+fengyewaitao.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 단풍잎 솜털 방한 미니 슈트</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>fengyewaitao.description</t>
   </si>
   <si>
     <t>由鼠族大师长眠生所定制的枫叶元素的保暖小西服，内部缝制毛绒打底，精致典雅而又温暖</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생이 제작한 내부에 솜털 안감을 덧대어 방한 성능을 높인 옷입니다. 멋과 보온성을 겸비했습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+beileimao.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생이 제작한 내부에 솜털 안감을 덧대어 방한 성능을 높인 옷입니다. 멋과 보온성을 겸비했습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>beileimao.label</t>
   </si>
   <si>
     <t>优雅贝雷帽</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 우아한 베레모</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+beileimao.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 우아한 베레모</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>beileimao.description</t>
   </si>
   <si>
     <t>维多利亚的大师们最喜欢的一种帽子，是贝雷帽的一种，精致优雅受人喜爱</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아의 장인들이 선호하는 모자입니다. 착용 시 약간의 사교 능력을 높여줍니다. 방어 능력은 거의 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+maorongdayi.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아의 장인들이 선호하는 모자입니다. 착용 시 약간의 사교 능력을 높여줍니다. 방어 능력은 거의 없습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>maorongdayi.label</t>
   </si>
   <si>
     <t>毛绒绒的风雪大衣</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 복슬복슬 방한 파카</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+maorongdayi.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 복슬복슬 방한 파카</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>maorongdayi.description</t>
   </si>
   <si>
     <t>精选动物毛发和皮绒制成的保暖大衣，毛绒绒的风雪大衣</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>엄선된 동물 털과 가죽으로 만든 방한 파카입니다. 극한의 추위 속에서도 체온을 유지하는 데 탁월합니다. 매우 복슬복슬합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+baonuanneiyi.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>엄선된 동물 털과 가죽으로 만든 방한 파카입니다. 극한의 추위 속에서도 체온을 유지하는 데 탁월합니다. 매우 복슬복슬합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>baonuanneiyi.label</t>
   </si>
   <si>
@@ -1980,105 +2006,105 @@
     <t>由鼠族大师长眠生所穿戴的保暖毛绒绒的保暖长衣</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생이 입었던 따뜻하고 복슬복슬한 롱코트입니다. 파카보다는 덜하지만 상당한 방한 성능을 제공합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kamz.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생이 입었던 따뜻하고 복슬복슬한 롱코트입니다. 파카보다는 덜하지만 상당한 방한 성능을 제공합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kamz.label</t>
   </si>
   <si>
     <t>可爱毛绒小羊帽</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 귀여운 솜털 양모자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kamz.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 귀여운 솜털 양모자</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kamz.description</t>
   </si>
   <si>
     <t>用保暖的棉花填充制成，可以包裹住整个头部和脖子，可爱的小羊角也是用保暖的材料填充，别指望它能头槌敌人</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>따뜻한 솜으로 채워 머리와 목 전체를 감싸주는 모자입니다. 귀여운 양 뿔이 달려있지만, 이걸로 박치기할 생각은 마십시오. 상당한 보온 효과를 제공합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xiaokb.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>따뜻한 솜으로 채워 머리와 목 전체를 감싸주는 모자입니다. 귀여운 양 뿔이 달려있지만, 이걸로 박치기할 생각은 마십시오. 상당한 보온 효과를 제공합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xiaokb.label</t>
   </si>
   <si>
     <t>皮革斜挎包</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>가죽 슬링백</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xiaokb.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>가죽 슬링백</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xiaokb.description</t>
   </si>
   <si>
     <t>鼠族大师长眠生斜挎的皮革包，里面可以装各种物资与装备，丝毫不影响携带者的动作</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생의 슬링백입니다. 일반 슬링백보다 조금 더 많은 물품을 휴대할 수 있으며, 착용자의 움직임을 방해하지 않습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+zsyg.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생의 슬링백입니다. 일반 슬링백보다 조금 더 많은 물품을 휴대할 수 있으며, 착용자의 움직임을 방해하지 않습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>zsyg.label</t>
   </si>
   <si>
@@ -2106,21 +2132,21 @@
     <t>一个腰带上面挂着很多小包，既可以放弹药，也可以放各种便携的东西，是鼠鼠们最常用的一种包</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>허리띠에 여러 개의 작은 주머니가 달린 가방입니다. 탄약이나 잡다한 휴대품을 넣기에 좋아 랫킨들이 애용합니다. 인간도 사용할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+yiliaob.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>허리띠에 여러 개의 작은 주머니가 달린 가방입니다. 탄약이나 잡다한 휴대품을 넣기에 좋아 랫킨들이 애용합니다. 인간도 사용할 수 있습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>yiliaob.label</t>
   </si>
   <si>
@@ -2139,21 +2165,21 @@
     <t>固定在腰部的医疗包。里面装有各种医疗物资。由于医疗包大小适合鼠族体型的缘故，对于人类而言医疗包太小了无法穿戴</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>허리에 고정하는 의료 가방입니다. 다양한 의료품이 들어있습니다. 랫킨의 체형에 맞춰 제작되어 인간은 착용하기에 너무 작습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+yingwu.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>허리에 고정하는 의료 가방입니다. 다양한 의료품이 들어있습니다. 랫킨의 체형에 맞춰 제작되어 인간은 착용하기에 너무 작습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>yingwu.label</t>
   </si>
   <si>
@@ -2184,405 +2210,405 @@
     <t>宫廷长裙</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 궁정 롱 드레스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwcq.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 궁정 롱 드레스</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwcq.description</t>
   </si>
   <si>
     <t>鼠族大师长眠生觐见女王时发现的雍容华贵白的发亮的内裙，与骑士团领主长裙同根同源</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생이 여왕 알현 시 보았던, 눈부시게 희고 화려한 드레스입니다. 기사단 영주 드레스와 뿌리가 같습니다. 사교적 영향력을 크게 높이지만, 활동에는 제약이 따릅니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwcqB.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생이 여왕 알현 시 보았던, 눈부시게 희고 화려한 드레스입니다. 기사단 영주 드레스와 뿌리가 같습니다. 사교적 영향력을 크게 높이지만, 활동에는 제약이 따릅니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwcqB.label</t>
   </si>
   <si>
     <t>宫廷长裙B款</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 궁정 롱 드레스 B형</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwcqB.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 궁정 롱 드레스 B형</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwcqB.description</t>
   </si>
   <si>
+    <t>ThingDef+nwpf.label</t>
+  </si>
+  <si>
     <t>nwpf.label</t>
   </si>
   <si>
-    <t>ThingDef+nwpf.label</t>
-  </si>
-  <si>
     <t>白湛女王披风</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 백광 여왕 망토</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwpf.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 백광 여왕 망토</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwpf.description</t>
   </si>
   <si>
     <t>鼠族大师长眠生觐见女王时发现的雍容华贵白的发亮的披风,她那白的发光的披风将穿戴者气质衬托的神圣尊贵，长长的衣摆即使拖在地上也不会沾染丝毫的灰尘</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 장인 장면생이 여왕 알현 시 보았던, 눈부시게 희고 화려한 망토입니다. 착용자에게 신성하고 고귀한 분위기를 더하며, 땅에 끌리는 긴 옷자락에도 먼지 하나 묻지 않습니다. 사교 능력과 약간의 정신적 보호 효과를 제공합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwtg.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 장인 장면생이 여왕 알현 시 보았던, 눈부시게 희고 화려한 망토입니다. 착용자에게 신성하고 고귀한 분위기를 더하며, 땅에 끌리는 긴 옷자락에도 먼지 하나 묻지 않습니다. 사교 능력과 약간의 정신적 보호 효과를 제공합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwtg.label</t>
   </si>
   <si>
     <t>灵能女王皇冠</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 초능력 여왕 왕관</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+nwtg.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 초능력 여왕 왕관</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>nwtg.description</t>
   </si>
   <si>
     <t>根据冠军侯甲胄内部的灵能符文篆刻技术，鼠族大师们用金子雕刻出来的高贵的头冠，灵能气息熠熠生辉</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>챔피언 후작 갑옷의 초능력 회로 각인 기술을 응용하여, 랫킨 장인들이 금으로 조각한 고귀한 왕관입니다. 초능력의 기운이 밝게 빛나며, 착용자의 정신 감응력과 엔트로피 최대치를 증가시킵니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+baonuanneiyi_Child.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>챔피언 후작 갑옷의 초능력 회로 각인 기술을 응용하여, 랫킨 장인들이 금으로 조각한 고귀한 왕관입니다. 초능력의 기운이 밝게 빛나며, 착용자의 정신 감응력과 엔트로피 최대치를 증가시킵니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>baonuanneiyi_Child.label</t>
   </si>
   <si>
     <t>儿童版毛绒绒长裙</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 랫킨 복슬복슬 롱 드레스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+baonuanneiyi_Child.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아동용 랫킨 복슬복슬 롱 드레스</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>baonuanneiyi_Child.description</t>
   </si>
   <si>
     <t>儿童版毛绒绒长裙.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아이들 크기에 맞춘 복슬복슬 롱 드레스입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+maorongdayi_Child.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아이들 크기에 맞춘 복슬복슬 롱 드레스입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>maorongdayi_Child.label</t>
   </si>
   <si>
     <t>儿童版毛绒绒大衣</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 랫킨 복슬복슬 파카</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+maorongdayi_Child.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아동용 랫킨 복슬복슬 파카</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>maorongdayi_Child.description</t>
   </si>
   <si>
     <t>儿童版毛绒绒大衣.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아이들 크기에 맞춘 복슬복슬 방한 파카입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kamz_Child.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아이들 크기에 맞춘 복슬복슬 방한 파카입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kamz_Child.label</t>
   </si>
   <si>
     <t>儿童版可爱毛绒小羊帽</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 랫킨 귀여운 솜털 양모자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kamz_Child.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아동용 랫킨 귀여운 솜털 양모자</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kamz_Child.description</t>
   </si>
   <si>
     <t>用保暖的棉花填充制成，可以包裹住整个头部和脖子，儿童版本</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아이들 크기에 맞춘 귀여운 솜털 양모자입니다. 따뜻한 솜으로 채워 머리와 목 전체를 감싸줍니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzj.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아이들 크기에 맞춘 귀여운 솜털 양모자입니다. 따뜻한 솜으로 채워 머리와 목 전체를 감싸줍니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzj.label</t>
   </si>
   <si>
     <t>纳米合金战甲（内甲）</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 나노 합금 갑옷 내의</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzj.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 나노 합금 갑옷 내의</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzj.description</t>
   </si>
   <si>
     <t>维多利亚科研机构根据无尽星芒技术开发的纳米级合金战斗装甲，由黄金、玻璃钢和铀制成的超导结构是战甲的主体，高昂的花费带来的是无与伦比的战力！神经纤维导体能够强化用户身体，发挥如超人般的力量与速度。其中内置的纳米修复机制能修复身体的各种损伤，凝结伤口加强细胞愈合，但并不能修复各种伤疤~</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 연구소가 '무한 성광' 기술로 개발한 나노 합금 갑옷의 내의입니다. 금, 유리강화섬유, 우라늄 기반 초전도 구조가 핵심입니다. 막대한 비용만큼 압도적인 전투력과 생존성을 보장합니다! 신경 섬유 전도체가 착용자의 신체를 강화하여 초인적인 힘과 속도를 부여합니다. 내장된 나노 수리 시스템은 신체 손상을 복구하고 상처를 봉합하며 세포 재생을 촉진하지만, 흉터까지 없애지는 못합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzjmz.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 연구소가 '무한 성광' 기술로 개발한 나노 합금 갑옷의 내의입니다. 금, 유리강화섬유, 우라늄 기반 초전도 구조가 핵심입니다. 막대한 비용만큼 압도적인 전투력과 생존성을 보장합니다! 신경 섬유 전도체가 착용자의 신체를 강화하여 초인적인 힘과 속도를 부여합니다. 내장된 나노 수리 시스템은 신체 손상을 복구하고 상처를 봉합하며 세포 재생을 촉진하지만, 흉터까지 없애지는 못합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzjmz.label</t>
   </si>
   <si>
     <t>纳米合金战甲面罩</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 나노 합금 헬멧</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzjmz.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 나노 합금 헬멧</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzjmz.description</t>
   </si>
   <si>
     <t>维多利亚科研机构根据人类挖掘的无尽星芒科技而开发的战甲面罩，神经纤维导体能够强化用户身体，内部由黄金与铀制作的高导体通路能够与大脑精密互通指导服务。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 연구소가 '무한 성광' 기술로 개발한 헬멧입니다. 신경 섬유 전도체가 착용자의 신체를 강화하며, 금과 우라늄으로 제작된 내부 고전도 회로가 뇌와 정밀하게 연결되어 조준 보조 및 전술 정보를 제공합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+gfzd.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 연구소가 '무한 성광' 기술로 개발한 헬멧입니다. 신경 섬유 전도체가 착용자의 신체를 강화하며, 금과 우라늄으로 제작된 내부 고전도 회로가 뇌와 정밀하게 연결되어 조준 보조 및 전술 정보를 제공합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>gfzd.label</t>
   </si>
   <si>
     <t>高分子剑刃</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>고분자검</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+gfzd.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>고분자검</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>gfzd.description</t>
   </si>
   <si>
     <t>纳米技术打造的高分子剑刃，在纳米分子的高速抖动下剑刃可以毫不费力的切开坚固的金属,维多利亚曾经向全世界出售过一批这种军武.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>나노 기술로 제작된 고분자검입니다. 나노 중합체의 고속 진동으로 단단한 금속 장갑도 손쉽게 절단합니다. 빅토리아는 과거 이 무기를 대량으로 판매한 적이 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+gfzd.tools.0.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>나노 기술로 제작된 고분자검입니다. 나노 중합체의 고속 진동으로 단단한 금속 장갑도 손쉽게 절단합니다. 빅토리아는 과거 이 무기를 대량으로 판매한 적이 있습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>gfzd.tools.0.label</t>
   </si>
   <si>
@@ -2625,237 +2651,237 @@
     <t>纳米合金战甲面罩B</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 나노 합금 헬멧 B형</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzjmzB.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 나노 합금 헬멧 B형</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzjmzB.description</t>
   </si>
   <si>
+    <t>ThingDef+hjzjwj.label</t>
+  </si>
+  <si>
     <t>hjzjwj.label</t>
   </si>
   <si>
-    <t>ThingDef+hjzjwj.label</t>
-  </si>
-  <si>
     <t>纳米合金战甲（外甲）</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 나노 합금 갑옷 외투</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+hjzjwj.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 나노 합금 갑옷 외투</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>hjzjwj.description</t>
   </si>
   <si>
     <t>维多利亚科研机构开发的纳米级合金战斗装甲，神经纤维导体能够强化用户身体，发挥如超人般的力量与速度,外部护甲拥有坚韧的防御，能够抵挡各种伤害而不影响用户剧烈活动</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 연구소가 개발한 나노 합금 갑옷의 외투입니다. 신경 섬유 전도체가 착용자의 신체를 강화하여 초인적인 힘과 속도를 부여합니다. 외부 장갑은 견고한 방어력을 제공하며, 격렬한 활동 중에도 착용자를 보호하고 움직임을 방해하지 않습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xqzzj.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 연구소가 개발한 나노 합금 갑옷의 외투입니다. 신경 섬유 전도체가 착용자의 신체를 강화하여 초인적인 힘과 속도를 부여합니다. 외부 장갑은 견고한 방어력을 제공하며, 격렬한 활동 중에도 착용자를 보호하고 움직임을 방해하지 않습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xqzzj.label</t>
   </si>
   <si>
     <t>先驱者战甲</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 선봉대 갑옷</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xqzzj.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 선봉대 갑옷</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xqzzj.description</t>
   </si>
   <si>
     <t>维多利亚科研机构应用先锋作战方针，牺牲部分防御护盾与功能来全面增强战甲的防护与机动力，简化的战甲在材料的应用效率更高，可以快速列装前线部队的增援能力。先驱者战甲内置极端天气抵御系统，可以在任意环境下作战</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 연구소가 작전 교리에 따라 개발한 전투복입니다. 방어막과 일부 기능을 희생하여 방호력과 기동성을 극대화했습니다. 간소화된 설계로 재료 효율을 높여 신속한 전선 배치가 가능합니다. 극한 환경 저항 시스템이 내장되어 어떤 환경에서도 작전 속행이 가능합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xqzmj.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 연구소가 작전 교리에 따라 개발한 전투복입니다. 방어막과 일부 기능을 희생하여 방호력과 기동성을 극대화했습니다. 간소화된 설계로 재료 효율을 높여 신속한 전선 배치가 가능합니다. 극한 환경 저항 시스템이 내장되어 어떤 환경에서도 작전 속행이 가능합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xqzmj.label</t>
   </si>
   <si>
     <t>先驱者作战面罩</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 선봉대 헬멧</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+xqzmj.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 선봉대 헬멧</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>xqzmj.description</t>
   </si>
   <si>
     <t>维多利亚科研机构应用先锋作战方针，牺牲部分防御护盾与功能来全面增强战甲的防护力与机动力，简化的战甲在材料的应用效率更高，可以快速列装前线部队的增援能力。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>선봉대 갑옷과 세트로 설계된 헬멧입니다. 방호력과 기동성에 중점을 뒀습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kydcmz.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>선봉대 갑옷과 세트로 설계된 헬멧입니다. 방호력과 기동성에 중점을 뒀습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kydcmz.label</t>
   </si>
   <si>
     <t>矿业调查面罩</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 광물 탐사장치</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kydcmz.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 광물 탐사장치</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kydcmz.description</t>
   </si>
   <si>
     <t>维多利亚矿业调查部门研发的AI实景调查装置，内部搭载深度求索AI，实时计算各种金属信息，提供各类开矿解决方案。</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 광업 조사부가 개발한 인공지능 조사장치입니다. 심층 탐색 AI가 내장되어 실시간으로 주변 광물 정보를 분석하고 최적의 채광 지점을 제안합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kydc.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 광업 조사부가 개발한 인공지능 조사장치입니다. 심층 탐색 AI가 내장되어 실시간으로 주변 광물 정보를 분석하고 최적의 채광 지점을 제안합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kydc.label</t>
   </si>
   <si>
     <t>矿业调查动力服</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 광물 채굴복</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+kydc.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>랫킨 광물 채굴복</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>kydc.description</t>
   </si>
   <si>
     <t>维多利亚矿业部门外派穿戴的专业服，运用先驱者设计理念，内嵌式动能骨骼能让使用者可以携带大量重物，节省用户体力，由于携带了最低限度的外方式的护盾，固无法穿戴其他服饰</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>빅토리아 광업부 외부 근로자용 작업복입니다. 선봉대 갑옷 기반의 내장형 동력장치가 착용자의 운반 능력을 향상시키고 피로도를 줄여줍니다. 최소한의 외부 보호 기능만 제공하며, 다른 겉옷과 함께 착용할 수 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThoughtDef+Happy.stages.0.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>빅토리아 광업부 외부 근로자용 작업복입니다. 선봉대 갑옷 기반의 내장형 동력장치가 착용자의 운반 능력을 향상시키고 피로도를 줄여줍니다. 최소한의 외부 보호 기능만 제공하며, 다른 겉옷과 함께 착용할 수 없습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>ThoughtDef</t>
   </si>
   <si>
@@ -2979,6 +3005,18 @@
     <t>ThingDef+bjq.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 귀족 롱 드레스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>bjq.description</t>
   </si>
   <si>
@@ -2988,6 +3026,18 @@
     <t>ThingDef+bjm.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 귀족 '천초·봉미선차'가 맞춤 제작한 옷입니다. 그녀는 언제나 손이 컸으며, 고성에 사는 귀족 같은 느낌을 물씬 풍깁니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>bjm.label</t>
   </si>
   <si>
@@ -2997,6 +3047,18 @@
     <t>ThingDef+bjm.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 귀족 레이스 머리장식</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>bjm.description</t>
   </si>
   <si>
@@ -3006,6 +3068,18 @@
     <t>DesignationCategoryDef+WDLY.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>랫킨 귀족 '천초·봉미선차'가 맞춤 제작한 머리장식입니다. 그녀는 언제나 손이 컸으며, 고성에 사는 귀족 같은 느낌을 물씬 풍깁니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DesignationCategoryDef</t>
   </si>
   <si>
@@ -3015,6 +3089,9 @@
     <t>维多利亚建筑</t>
   </si>
   <si>
+    <t>빅토리아풍 건축물</t>
+  </si>
+  <si>
     <t>ThingDef+ch.label</t>
   </si>
   <si>
@@ -3024,6 +3101,9 @@
     <t>精致阳台窗</t>
   </si>
   <si>
+    <t>정교한 발코니 창문</t>
+  </si>
+  <si>
     <t>ThingDef+ch.description</t>
   </si>
   <si>
@@ -3033,6 +3113,9 @@
     <t>维多利亚特色建筑的精致阳台窗</t>
   </si>
   <si>
+    <t>빅토리아 양식 특유의 정교한 발코니 창문입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+xzz.label</t>
   </si>
   <si>
@@ -3045,6 +3128,18 @@
     <t>ThingDef+xzz.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>정교한 작은 책상 (1x1)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>xzz.description</t>
   </si>
   <si>
@@ -3054,27 +3149,45 @@
     <t>ThingDef+xzzB.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>클래식한 스타일의 작은 책상으로, 식사나 데이트에 좋은 선택입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>xzzB.label</t>
   </si>
   <si>
     <t>精致小桌B(1x1)</t>
   </si>
   <si>
+    <t>정교한 작은 책상 B (1x1)</t>
+  </si>
+  <si>
     <t>ThingDef+xzzB.description</t>
   </si>
   <si>
     <t>xzzB.description</t>
   </si>
   <si>
+    <t>xyz.label</t>
+  </si>
+  <si>
     <t>ThingDef+xyz.label</t>
   </si>
   <si>
-    <t>xyz.label</t>
-  </si>
-  <si>
     <t>欧式沙发椅</t>
   </si>
   <si>
+    <t>유럽풍 소파 의자</t>
+  </si>
+  <si>
     <t>ThingDef+xyz.description</t>
   </si>
   <si>
@@ -3084,6 +3197,9 @@
     <t>精致的沙发椅子</t>
   </si>
   <si>
+    <t>정교한 소파 의자입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+dt.label</t>
   </si>
   <si>
@@ -3093,6 +3209,9 @@
     <t>精美圆型地毯</t>
   </si>
   <si>
+    <t>정교한 원형 카펫</t>
+  </si>
+  <si>
     <t>ThingDef+dt.description</t>
   </si>
   <si>
@@ -3102,51 +3221,188 @@
     <t>精美圆型地毯，用金丝勾画的精美图案。通过旋转控制地毯的位置</t>
   </si>
   <si>
-    <t>빅토리아풍 건축물</t>
-  </si>
-  <si>
-    <t>정교한 발코니 창문</t>
-  </si>
-  <si>
-    <t>빅토리아 양식 특유의 정교한 발코니 창문입니다.</t>
-  </si>
-  <si>
-    <t>유럽풍 소파 의자</t>
-  </si>
-  <si>
-    <t>정교한 소파 의자입니다.</t>
-  </si>
-  <si>
-    <t>정교한 원형 카펫</t>
-  </si>
-  <si>
     <t>정교한 원형 카펫입니다. 금실로 아름다운 문양을 수놓았습니다. 회전하여 카펫의 위치를 조절할 수 있습니다.</t>
   </si>
   <si>
-    <t>랫킨 귀족 롱 드레스</t>
+    <t>ThingDef+FBZX.label</t>
+  </si>
+  <si>
+    <t>FBZX.label</t>
+  </si>
+  <si>
+    <t>无尽之息</t>
+  </si>
+  <si>
+    <t>ThingDef+FBZX.description</t>
+  </si>
+  <si>
+    <t>FBZX.description</t>
+  </si>
+  <si>
+    <t>来自无尽科技武器系列，维多利亚科研天才们改进了枪身，适应鼠族人体工学机能，内部多重光纤磁道加强穿甲能力的同时还减少后座，光储能子弹能让人体分子层运转骤停</t>
+  </si>
+  <si>
+    <t>ThingDef+FBZX.verbs.Verb_Shoot.label</t>
+  </si>
+  <si>
+    <t>FBZX.verbs.Verb_Shoot.label</t>
+  </si>
+  <si>
+    <t>ThingDef+FBZX.tools.0.label</t>
+  </si>
+  <si>
+    <t>FBZX.tools.0.label</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>ThingDef+FBZX.tools.1.label</t>
+  </si>
+  <si>
+    <t>FBZX.tools.1.label</t>
+  </si>
+  <si>
+    <t>barrel</t>
+  </si>
+  <si>
+    <t>ThingDef+LightbulletA.label</t>
+  </si>
+  <si>
+    <t>LightbulletA.label</t>
+  </si>
+  <si>
+    <t>光储能弹</t>
+  </si>
+  <si>
+    <t>ThingCategoryDef+AmmoLightbulletA.label</t>
+  </si>
+  <si>
+    <t>ThingCategoryDef</t>
+  </si>
+  <si>
+    <t>AmmoLightbulletA.label</t>
+  </si>
+  <si>
+    <t>鼠族光储能弹</t>
+  </si>
+  <si>
+    <t>CombatExtended.AmmoSetDef+AmmoSet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>CombatExtended.AmmoSetDef</t>
+  </si>
+  <si>
+    <t>AmmoSet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>鼠族光储能弹弹药</t>
+  </si>
+  <si>
+    <t>ThingDef+AmmoSet_LightbulletA.description</t>
+  </si>
+  <si>
+    <t>AmmoSet_LightbulletA.description</t>
+  </si>
+  <si>
+    <t>制造的用于鼠族无尽之息武器的光裂变穿甲射击弹药.</t>
+  </si>
+  <si>
+    <t>ThingDef+AmmoSet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Bullet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>Bullet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>RecipeDef+MakeAmmoSet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>RecipeDef</t>
+  </si>
+  <si>
+    <t>MakeAmmoSet_LightbulletA.label</t>
+  </si>
+  <si>
+    <t>制作500发鼠族光储能弹弹药</t>
+  </si>
+  <si>
+    <t>RecipeDef+MakeAmmoSet_LightbulletA.description</t>
+  </si>
+  <si>
+    <t>MakeAmmoSet_LightbulletA.description</t>
+  </si>
+  <si>
+    <t>制作500鼠族光储能弹弹药.</t>
+  </si>
+  <si>
+    <t>RecipeDef+MakeAmmoSet_LightbulletA.jobString</t>
+  </si>
+  <si>
+    <t>MakeAmmoSet_LightbulletA.jobString</t>
+  </si>
+  <si>
+    <t>制作500光鼠族光储能弹.</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+FBZX.tools.0.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+FBZX.tools.1.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+FBZX.tools.2.label</t>
+  </si>
+  <si>
+    <t>FBZX.tools.2.label</t>
+  </si>
+  <si>
+    <t>muzzle</t>
+  </si>
+  <si>
+    <t>무한의 숨결</t>
+  </si>
+  <si>
+    <t>개머리판</t>
+  </si>
+  <si>
+    <t>총열</t>
+  </si>
+  <si>
+    <t>총열</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>랫킨 귀족 '천초·봉미선차'가 맞춤 제작한 옷입니다. 그녀는 언제나 손이 컸으며, 고성에 사는 귀족 같은 느낌을 물씬 풍깁니다.</t>
+    <t>총구</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>랫킨 귀족 레이스 머리장식</t>
+    <t>태양광 집전탄</t>
+  </si>
+  <si>
+    <t>랫킨 태양광 집전탄</t>
+  </si>
+  <si>
+    <t>랫킨 '무한의 숨결' 무기에 사용하기 위해 제조된 광분열 장갑 관통형 탄약입니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>랫킨 귀족 '천초·봉미선차'가 맞춤 제작한 머리장식입니다. 그녀는 언제나 손이 컸으며, 고성에 사는 귀족 같은 느낌을 물씬 풍깁니다.</t>
+    <t>랫킨 태양광 탄약</t>
+  </si>
+  <si>
+    <t>랫킨 태양광 탄약 만들기 (x500)</t>
+  </si>
+  <si>
+    <t>랫킨 태양광 탄약을 만듭니다.</t>
+  </si>
+  <si>
+    <t>랫킨 태양광 탄약 만드는 중</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>정교한 작은 책상 B (1x1)</t>
-  </si>
-  <si>
-    <t>클래식한 스타일의 작은 책상으로, 식사나 데이트에 좋은 선택입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>정교한 작은 책상 (1x1)</t>
+    <t>빅토리아의 천재 과학자들이 무한 성광 무기를 랫킨에 맞게 개량했습니다. 내부 다중 광섬유 자기 총열은 장갑 관통력을 강화하는 동시에 반동을 줄이며, 태양광 탄약은 인체 분자층의 움직임을 급정지시킬 수 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3538,10 +3794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="J114" sqref="J114"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3771,12 +4027,12 @@
         <v>54</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>48</v>
@@ -3805,12 +4061,12 @@
         <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
@@ -3839,12 +4095,12 @@
         <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -3907,12 +4163,12 @@
         <v>86</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>48</v>
@@ -3958,12 +4214,12 @@
         <v>98</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>48</v>
@@ -3992,12 +4248,12 @@
         <v>106</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>48</v>
@@ -4043,12 +4299,12 @@
         <v>119</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>117</v>
@@ -4060,12 +4316,12 @@
         <v>123</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>126</v>
@@ -4111,12 +4367,12 @@
         <v>136</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
@@ -4128,12 +4384,12 @@
         <v>140</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -4145,12 +4401,12 @@
         <v>144</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
@@ -4162,12 +4418,12 @@
         <v>148</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -4179,12 +4435,12 @@
         <v>152</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -4196,12 +4452,12 @@
         <v>156</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
@@ -4213,12 +4469,12 @@
         <v>160</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -4230,12 +4486,12 @@
         <v>164</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
@@ -4264,12 +4520,12 @@
         <v>172</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
@@ -4281,12 +4537,12 @@
         <v>176</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
@@ -4298,12 +4554,12 @@
         <v>180</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
@@ -4315,12 +4571,12 @@
         <v>184</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
@@ -4332,12 +4588,12 @@
         <v>188</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
@@ -4366,12 +4622,12 @@
         <v>196</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -4400,12 +4656,12 @@
         <v>204</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
@@ -4451,12 +4707,12 @@
         <v>216</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>7</v>
@@ -4468,12 +4724,12 @@
         <v>220</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>7</v>
@@ -4485,12 +4741,12 @@
         <v>224</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
@@ -4502,29 +4758,29 @@
         <v>220</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>230</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>7</v>
@@ -4536,12 +4792,12 @@
         <v>234</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>7</v>
@@ -4553,12 +4809,12 @@
         <v>238</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
@@ -4570,12 +4826,12 @@
         <v>242</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>7</v>
@@ -4587,12 +4843,12 @@
         <v>246</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
@@ -4604,12 +4860,12 @@
         <v>250</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>7</v>
@@ -4621,12 +4877,12 @@
         <v>254</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>7</v>
@@ -4638,12 +4894,12 @@
         <v>258</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
@@ -4655,12 +4911,12 @@
         <v>262</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
@@ -4672,12 +4928,12 @@
         <v>266</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
@@ -4689,12 +4945,12 @@
         <v>270</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
@@ -4706,12 +4962,12 @@
         <v>274</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>7</v>
@@ -4723,12 +4979,12 @@
         <v>278</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
@@ -4740,12 +4996,12 @@
         <v>282</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>7</v>
@@ -4757,12 +5013,12 @@
         <v>286</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>7</v>
@@ -4774,12 +5030,12 @@
         <v>290</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>7</v>
@@ -4842,12 +5098,12 @@
         <v>306</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>7</v>
@@ -4859,29 +5115,29 @@
         <v>282</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>312</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>7</v>
@@ -4893,12 +5149,12 @@
         <v>316</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
@@ -4910,12 +5166,12 @@
         <v>320</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>7</v>
@@ -4927,12 +5183,12 @@
         <v>324</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
@@ -4944,12 +5200,12 @@
         <v>328</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>7</v>
@@ -4961,12 +5217,12 @@
         <v>332</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>7</v>
@@ -4978,12 +5234,12 @@
         <v>336</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>7</v>
@@ -4995,12 +5251,12 @@
         <v>340</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>7</v>
@@ -5012,12 +5268,12 @@
         <v>344</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>7</v>
@@ -5029,12 +5285,12 @@
         <v>348</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>351</v>
@@ -5242,7 +5498,7 @@
         <v>390</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>440</v>
+        <v>392</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
@@ -5253,234 +5509,556 @@
         <v>7</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>442</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>443</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>446</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>439</v>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A118" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A119" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A120" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A131" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>